<commit_message>
test(adm/cmd): test export data
</commit_message>
<xml_diff>
--- a/cmd/containers.xlsx
+++ b/cmd/containers.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Container Name</t>
   </si>
@@ -28,28 +28,16 @@
     <t>nginx:latest</t>
   </si>
   <si>
-    <t>redis-container-1</t>
-  </si>
-  <si>
-    <t>redis:alpine</t>
-  </si>
-  <si>
-    <t>postgres-container-1</t>
-  </si>
-  <si>
-    <t>postgres:13</t>
-  </si>
-  <si>
-    <t>ubuntu-container-1</t>
-  </si>
-  <si>
-    <t>ubuntu:20.04</t>
-  </si>
-  <si>
-    <t>mysql-container-1</t>
-  </si>
-  <si>
-    <t>mysql:8.0</t>
+    <t>nginx-container-2</t>
+  </si>
+  <si>
+    <t>nginx-container-3</t>
+  </si>
+  <si>
+    <t>nginx-container-4</t>
+  </si>
+  <si>
+    <t>nginx-container-5</t>
   </si>
 </sst>
 </file>
@@ -380,31 +368,31 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>